<commit_message>
add max and min to summary table
</commit_message>
<xml_diff>
--- a/SAS/mean_sem.xlsx
+++ b/SAS/mean_sem.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,21 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>max</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>min_non_zero</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>letter_group</t>
         </is>
       </c>
@@ -465,9 +480,18 @@
         <v>0.8198198198198198</v>
       </c>
       <c r="C2" t="n">
-        <v>0.03664513893725976</v>
-      </c>
-      <c r="D2" t="inlineStr">
+        <v>0.03664513893725978</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>a</t>
         </is>
@@ -483,9 +507,18 @@
         <v>0.05405405405405406</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02156010905993149</v>
-      </c>
-      <c r="D3" t="inlineStr">
+        <v>0.0215601090599315</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -501,9 +534,18 @@
         <v>0.009009009009009009</v>
       </c>
       <c r="C4" t="n">
-        <v>0.009009009009009018</v>
-      </c>
-      <c r="D4" t="inlineStr">
+        <v>0.009009009009009011</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -519,9 +561,18 @@
         <v>0.09009009009009009</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02729866226453558</v>
-      </c>
-      <c r="D5" t="inlineStr">
+        <v>0.02729866226453556</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -537,9 +588,18 @@
         <v>0.009009009009009009</v>
       </c>
       <c r="C6" t="n">
-        <v>0.009009009009009019</v>
-      </c>
-      <c r="D6" t="inlineStr">
+        <v>0.009009009009009011</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -555,9 +615,18 @@
         <v>0.009009009009009009</v>
       </c>
       <c r="C7" t="n">
-        <v>0.009009009009009012</v>
-      </c>
-      <c r="D7" t="inlineStr">
+        <v>0.009009009009009011</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -575,7 +644,16 @@
       <c r="C8" t="n">
         <v>0.009009009009009011</v>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -591,9 +669,18 @@
         <v>109.8738738738739</v>
       </c>
       <c r="C9" t="n">
-        <v>22.76734200418762</v>
-      </c>
-      <c r="D9" t="inlineStr">
+        <v>22.76734200418761</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1520</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>a</t>
         </is>
@@ -611,7 +698,16 @@
       <c r="C10" t="n">
         <v>11.69436944449006</v>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" t="n">
+        <v>1296</v>
+      </c>
+      <c r="E10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -627,9 +723,18 @@
         <v>4.207207207207207</v>
       </c>
       <c r="C11" t="n">
-        <v>4.207207207207211</v>
-      </c>
-      <c r="D11" t="inlineStr">
+        <v>4.207207207207208</v>
+      </c>
+      <c r="D11" t="n">
+        <v>467</v>
+      </c>
+      <c r="E11" t="n">
+        <v>467</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>bc</t>
         </is>
@@ -645,9 +750,18 @@
         <v>9.36936936936937</v>
       </c>
       <c r="C12" t="n">
-        <v>4.714935718036187</v>
-      </c>
-      <c r="D12" t="inlineStr">
+        <v>4.714935718036188</v>
+      </c>
+      <c r="D12" t="n">
+        <v>424</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>b</t>
         </is>
@@ -663,9 +777,18 @@
         <v>0.06306306306306306</v>
       </c>
       <c r="C13" t="n">
-        <v>0.06306306306306299</v>
-      </c>
-      <c r="D13" t="inlineStr">
+        <v>0.06306306306306306</v>
+      </c>
+      <c r="D13" t="n">
+        <v>7</v>
+      </c>
+      <c r="E13" t="n">
+        <v>7</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>e</t>
         </is>
@@ -681,9 +804,18 @@
         <v>0.9099099099099099</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9099099099099097</v>
-      </c>
-      <c r="D14" t="inlineStr">
+        <v>0.9099099099099099</v>
+      </c>
+      <c r="D14" t="n">
+        <v>101</v>
+      </c>
+      <c r="E14" t="n">
+        <v>101</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t>cd</t>
         </is>
@@ -701,7 +833,16 @@
       <c r="C15" t="n">
         <v>0.1891891891891892</v>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" t="n">
+        <v>21</v>
+      </c>
+      <c r="E15" t="n">
+        <v>21</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="inlineStr">
         <is>
           <t>de</t>
         </is>

</xml_diff>